<commit_message>
Atualizado por script em 25-10-2023 12:32
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V59"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5885,6 +5885,190 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>45224.54166666666</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Alashkert</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>BKMA</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>24/10/2023 00:12</t>
+        </is>
+      </c>
+      <c r="L60" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>25/10/2023 12:51</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>24/10/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P60" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>25/10/2023 12:51</t>
+        </is>
+      </c>
+      <c r="R60" t="n">
+        <v>7.01</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>24/10/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T60" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>25/10/2023 12:51</t>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/alashkert-bkma/0Czsnty8/</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>45224.54166666666</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Pyunik Yerevan</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>3</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>24/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L61" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>25/10/2023 12:58</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>24/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P61" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>25/10/2023 12:58</t>
+        </is>
+      </c>
+      <c r="R61" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>24/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T61" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>25/10/2023 12:58</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-urartu/tCTUlrik/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 26-10-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6069,6 +6069,98 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>45225.70833333334</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Shirak Gyumri</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>2</v>
+      </c>
+      <c r="J62" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>25/10/2023 04:14</t>
+        </is>
+      </c>
+      <c r="L62" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>26/10/2023 16:59</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>25/10/2023 04:14</t>
+        </is>
+      </c>
+      <c r="P62" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>26/10/2023 16:59</t>
+        </is>
+      </c>
+      <c r="R62" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>25/10/2023 04:14</t>
+        </is>
+      </c>
+      <c r="T62" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>26/10/2023 16:59</t>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/shirak-gyumri-noah/EFOOAPD8/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 31-10-2023 15:01
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V62"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6161,6 +6161,466 @@
         </is>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>45227.54166666666</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Ararat-Armenia</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>2</v>
+      </c>
+      <c r="J63" t="n">
+        <v>8</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L63" t="n">
+        <v>10.13</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>28/10/2023 12:26</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>5.29</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P63" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>28/10/2023 12:26</t>
+        </is>
+      </c>
+      <c r="R63" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T63" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>28/10/2023 12:26</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/van-ararat-armenia/tUv5jeSg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>45228.45833333334</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>West Armenia</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>2</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Pyunik Yerevan</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>3</v>
+      </c>
+      <c r="J64" t="n">
+        <v>30.52</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>29/10/2023 06:14</t>
+        </is>
+      </c>
+      <c r="L64" t="n">
+        <v>30.52</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>29/10/2023 06:14</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>16.62</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>29/10/2023 06:14</t>
+        </is>
+      </c>
+      <c r="P64" t="n">
+        <v>16.62</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>29/10/2023 06:14</t>
+        </is>
+      </c>
+      <c r="R64" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>29/10/2023 06:14</t>
+        </is>
+      </c>
+      <c r="T64" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>29/10/2023 06:14</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/west-armenia-pyunik-yerevan/fXr9kFs0/</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>45228.58333333334</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>BKMA</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>2</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Ararat Yerevan</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>28/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L65" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>29/10/2023 13:52</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>28/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P65" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>29/10/2023 13:52</t>
+        </is>
+      </c>
+      <c r="R65" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>28/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T65" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>29/10/2023 13:52</t>
+        </is>
+      </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/bkma-ararat-yerevan/n7u1iyDm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>45229.58333333334</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>4</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Alashkert</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>2</v>
+      </c>
+      <c r="J66" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>29/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L66" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>30/10/2023 13:59</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>29/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P66" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>30/10/2023 13:59</t>
+        </is>
+      </c>
+      <c r="R66" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>29/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T66" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>30/10/2023 13:59</t>
+        </is>
+      </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/noah-alashkert/8GtchHcs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>45229.66666666666</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>2</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Shirak Gyumri</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>2</v>
+      </c>
+      <c r="J67" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>29/10/2023 04:12</t>
+        </is>
+      </c>
+      <c r="L67" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>30/10/2023 15:43</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>29/10/2023 04:12</t>
+        </is>
+      </c>
+      <c r="P67" t="n">
+        <v>5.37</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>30/10/2023 15:59</t>
+        </is>
+      </c>
+      <c r="R67" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>29/10/2023 04:12</t>
+        </is>
+      </c>
+      <c r="T67" t="n">
+        <v>9.91</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>30/10/2023 15:59</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/urartu-shirak-gyumri/h6NS9qTE/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 02-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V67"/>
+  <dimension ref="A1:V69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6621,6 +6621,190 @@
         </is>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>45232.45833333334</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Pyunik Yerevan</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>6</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L68" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>02/11/2023 10:13</t>
+        </is>
+      </c>
+      <c r="N68" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P68" t="n">
+        <v>9.949999999999999</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>02/11/2023 10:56</t>
+        </is>
+      </c>
+      <c r="R68" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T68" t="n">
+        <v>19.88</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>02/11/2023 10:56</t>
+        </is>
+      </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-van/GnXHmgCC/</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>45232.625</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Ararat-Armenia</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>4</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>BKMA</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>01/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L69" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>02/11/2023 14:54</t>
+        </is>
+      </c>
+      <c r="N69" t="n">
+        <v>6.44</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>01/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P69" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>02/11/2023 14:55</t>
+        </is>
+      </c>
+      <c r="R69" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>01/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T69" t="n">
+        <v>16.18</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>02/11/2023 14:55</t>
+        </is>
+      </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/ararat-armenia-bkma/OCWLnDRI/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 03-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V69"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6805,6 +6805,98 @@
         </is>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>45233.54166666666</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>West Armenia</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>2</v>
+      </c>
+      <c r="J70" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>03/11/2023 11:27</t>
+        </is>
+      </c>
+      <c r="L70" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>03/11/2023 11:27</t>
+        </is>
+      </c>
+      <c r="N70" t="n">
+        <v>17.67</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>03/11/2023 11:30</t>
+        </is>
+      </c>
+      <c r="P70" t="n">
+        <v>17.67</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>03/11/2023 11:30</t>
+        </is>
+      </c>
+      <c r="R70" t="n">
+        <v>27.78</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>03/11/2023 11:30</t>
+        </is>
+      </c>
+      <c r="T70" t="n">
+        <v>27.78</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>03/11/2023 11:30</t>
+        </is>
+      </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/urartu-west-armenia/xdYDlZd6/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 03-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5449,22 +5449,22 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Pyunik Yerevan</t>
+          <t>Van</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Ararat-Armenia</t>
+          <t>Alashkert</t>
         </is>
       </c>
       <c r="I55" t="n">
         <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>1.85</v>
+        <v>6.34</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -5472,7 +5472,7 @@
         </is>
       </c>
       <c r="L55" t="n">
-        <v>1.99</v>
+        <v>7.32</v>
       </c>
       <c r="M55" t="inlineStr">
         <is>
@@ -5480,7 +5480,7 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>3.41</v>
+        <v>4.55</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -5488,7 +5488,7 @@
         </is>
       </c>
       <c r="P55" t="n">
-        <v>3.24</v>
+        <v>4.51</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -5496,7 +5496,7 @@
         </is>
       </c>
       <c r="R55" t="n">
-        <v>3.73</v>
+        <v>1.38</v>
       </c>
       <c r="S55" t="inlineStr">
         <is>
@@ -5504,7 +5504,7 @@
         </is>
       </c>
       <c r="T55" t="n">
-        <v>3.39</v>
+        <v>1.43</v>
       </c>
       <c r="U55" t="inlineStr">
         <is>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
         </is>
       </c>
     </row>
@@ -5541,22 +5541,22 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Van</t>
+          <t>Pyunik Yerevan</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Alashkert</t>
+          <t>Ararat-Armenia</t>
         </is>
       </c>
       <c r="I56" t="n">
         <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>6.34</v>
+        <v>1.85</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -5564,7 +5564,7 @@
         </is>
       </c>
       <c r="L56" t="n">
-        <v>7.32</v>
+        <v>1.99</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>4.55</v>
+        <v>3.41</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -5580,7 +5580,7 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>4.51</v>
+        <v>3.24</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -5588,7 +5588,7 @@
         </is>
       </c>
       <c r="R56" t="n">
-        <v>1.38</v>
+        <v>3.73</v>
       </c>
       <c r="S56" t="inlineStr">
         <is>
@@ -5596,7 +5596,7 @@
         </is>
       </c>
       <c r="T56" t="n">
-        <v>1.43</v>
+        <v>3.39</v>
       </c>
       <c r="U56" t="inlineStr">
         <is>
@@ -5605,7 +5605,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
         </is>
       </c>
     </row>
@@ -6894,6 +6894,98 @@
       <c r="V70" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/armenia/premier-league/urartu-west-armenia/xdYDlZd6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>45233.625</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Ararat Yerevan</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>2</v>
+      </c>
+      <c r="J71" t="n">
+        <v>5.54</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>02/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L71" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>03/11/2023 14:59</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>02/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P71" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>03/11/2023 14:59</t>
+        </is>
+      </c>
+      <c r="R71" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>02/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T71" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>03/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/ararat-yerevan-noah/23VPoXtP/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 07-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V73"/>
+  <dimension ref="A1:V74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7173,6 +7173,98 @@
         </is>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>45237.625</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Ararat-Armenia</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>06/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L74" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>07/11/2023 14:55</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>06/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P74" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>07/11/2023 14:58</t>
+        </is>
+      </c>
+      <c r="R74" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>06/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T74" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>07/11/2023 14:58</t>
+        </is>
+      </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/noah-ararat-armenia/ADdhtgKh/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 08-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V74"/>
+  <dimension ref="A1:V75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5449,22 +5449,22 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Van</t>
+          <t>Pyunik Yerevan</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Alashkert</t>
+          <t>Ararat-Armenia</t>
         </is>
       </c>
       <c r="I55" t="n">
         <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>6.34</v>
+        <v>1.85</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -5472,7 +5472,7 @@
         </is>
       </c>
       <c r="L55" t="n">
-        <v>7.32</v>
+        <v>1.99</v>
       </c>
       <c r="M55" t="inlineStr">
         <is>
@@ -5480,7 +5480,7 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>4.55</v>
+        <v>3.41</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -5488,7 +5488,7 @@
         </is>
       </c>
       <c r="P55" t="n">
-        <v>4.51</v>
+        <v>3.24</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -5496,7 +5496,7 @@
         </is>
       </c>
       <c r="R55" t="n">
-        <v>1.38</v>
+        <v>3.73</v>
       </c>
       <c r="S55" t="inlineStr">
         <is>
@@ -5504,7 +5504,7 @@
         </is>
       </c>
       <c r="T55" t="n">
-        <v>1.43</v>
+        <v>3.39</v>
       </c>
       <c r="U55" t="inlineStr">
         <is>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
         </is>
       </c>
     </row>
@@ -5541,22 +5541,22 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Pyunik Yerevan</t>
+          <t>Van</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Ararat-Armenia</t>
+          <t>Alashkert</t>
         </is>
       </c>
       <c r="I56" t="n">
         <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>1.85</v>
+        <v>6.34</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -5564,7 +5564,7 @@
         </is>
       </c>
       <c r="L56" t="n">
-        <v>1.99</v>
+        <v>7.32</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>3.41</v>
+        <v>4.55</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -5580,7 +5580,7 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>3.24</v>
+        <v>4.51</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -5588,7 +5588,7 @@
         </is>
       </c>
       <c r="R56" t="n">
-        <v>3.73</v>
+        <v>1.38</v>
       </c>
       <c r="S56" t="inlineStr">
         <is>
@@ -5596,7 +5596,7 @@
         </is>
       </c>
       <c r="T56" t="n">
-        <v>3.39</v>
+        <v>1.43</v>
       </c>
       <c r="U56" t="inlineStr">
         <is>
@@ -5605,7 +5605,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
         </is>
       </c>
     </row>
@@ -7262,6 +7262,98 @@
       <c r="V74" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/armenia/premier-league/noah-ararat-armenia/ADdhtgKh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>45238.54166666666</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Shirak Gyumri</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Ararat Yerevan</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>2</v>
+      </c>
+      <c r="J75" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>07/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L75" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>08/11/2023 12:55</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v>3</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>07/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P75" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>08/11/2023 12:59</t>
+        </is>
+      </c>
+      <c r="R75" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>07/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T75" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>08/11/2023 12:54</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/shirak-gyumri-ararat-yerevan/WMclsZ4n/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 08-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V75"/>
+  <dimension ref="A1:V76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5449,22 +5449,22 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Pyunik Yerevan</t>
+          <t>Van</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Ararat-Armenia</t>
+          <t>Alashkert</t>
         </is>
       </c>
       <c r="I55" t="n">
         <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>1.85</v>
+        <v>6.34</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -5472,7 +5472,7 @@
         </is>
       </c>
       <c r="L55" t="n">
-        <v>1.99</v>
+        <v>7.32</v>
       </c>
       <c r="M55" t="inlineStr">
         <is>
@@ -5480,7 +5480,7 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>3.41</v>
+        <v>4.55</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -5488,7 +5488,7 @@
         </is>
       </c>
       <c r="P55" t="n">
-        <v>3.24</v>
+        <v>4.51</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -5496,7 +5496,7 @@
         </is>
       </c>
       <c r="R55" t="n">
-        <v>3.73</v>
+        <v>1.38</v>
       </c>
       <c r="S55" t="inlineStr">
         <is>
@@ -5504,7 +5504,7 @@
         </is>
       </c>
       <c r="T55" t="n">
-        <v>3.39</v>
+        <v>1.43</v>
       </c>
       <c r="U55" t="inlineStr">
         <is>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
         </is>
       </c>
     </row>
@@ -5541,22 +5541,22 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Van</t>
+          <t>Pyunik Yerevan</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Alashkert</t>
+          <t>Ararat-Armenia</t>
         </is>
       </c>
       <c r="I56" t="n">
         <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>6.34</v>
+        <v>1.85</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -5564,7 +5564,7 @@
         </is>
       </c>
       <c r="L56" t="n">
-        <v>7.32</v>
+        <v>1.99</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>4.55</v>
+        <v>3.41</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -5580,7 +5580,7 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>4.51</v>
+        <v>3.24</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -5588,7 +5588,7 @@
         </is>
       </c>
       <c r="R56" t="n">
-        <v>1.38</v>
+        <v>3.73</v>
       </c>
       <c r="S56" t="inlineStr">
         <is>
@@ -5596,7 +5596,7 @@
         </is>
       </c>
       <c r="T56" t="n">
-        <v>1.43</v>
+        <v>3.39</v>
       </c>
       <c r="U56" t="inlineStr">
         <is>
@@ -5605,7 +5605,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
         </is>
       </c>
     </row>
@@ -7354,6 +7354,98 @@
       <c r="V75" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/armenia/premier-league/shirak-gyumri-ararat-yerevan/WMclsZ4n/</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>45238.66666666666</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Alashkert</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>07/11/2023 04:12</t>
+        </is>
+      </c>
+      <c r="L76" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>08/11/2023 15:58</t>
+        </is>
+      </c>
+      <c r="N76" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>07/11/2023 04:12</t>
+        </is>
+      </c>
+      <c r="P76" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>08/11/2023 15:58</t>
+        </is>
+      </c>
+      <c r="R76" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>07/11/2023 04:12</t>
+        </is>
+      </c>
+      <c r="T76" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>08/11/2023 15:58</t>
+        </is>
+      </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/urartu-alashkert/x0bprFkt/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 11-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:V77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7449,6 +7449,98 @@
         </is>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>45241.5</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Pyunik Yerevan</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>3</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>10/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="L77" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>11/11/2023 10:23</t>
+        </is>
+      </c>
+      <c r="N77" t="n">
+        <v>4.35</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>10/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P77" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>11/11/2023 11:04</t>
+        </is>
+      </c>
+      <c r="R77" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>10/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T77" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>11/11/2023 11:04</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-noah/f1rEyVYN/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 12-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V78"/>
+  <dimension ref="A1:V79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5909,71 +5909,71 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Alashkert</t>
+          <t>Pyunik Yerevan</t>
         </is>
       </c>
       <c r="G60" t="n">
+        <v>3</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
         <v>1</v>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>BKMA</t>
-        </is>
-      </c>
-      <c r="I60" t="n">
-        <v>0</v>
-      </c>
       <c r="J60" t="n">
-        <v>1.33</v>
+        <v>1.66</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>24/10/2023 00:12</t>
+          <t>24/10/2023 03:12</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>1.36</v>
+        <v>1.61</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>25/10/2023 12:51</t>
+          <t>25/10/2023 12:58</t>
         </is>
       </c>
       <c r="N60" t="n">
-        <v>4.78</v>
+        <v>3.7</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>24/10/2023 00:12</t>
+          <t>24/10/2023 03:12</t>
         </is>
       </c>
       <c r="P60" t="n">
-        <v>4.99</v>
+        <v>3.92</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>25/10/2023 12:51</t>
+          <t>25/10/2023 12:58</t>
         </is>
       </c>
       <c r="R60" t="n">
-        <v>7.01</v>
+        <v>4.36</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>24/10/2023 00:12</t>
+          <t>24/10/2023 03:12</t>
         </is>
       </c>
       <c r="T60" t="n">
-        <v>8.109999999999999</v>
+        <v>5.58</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>25/10/2023 12:51</t>
+          <t>25/10/2023 12:58</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/alashkert-bkma/0Czsnty8/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-urartu/tCTUlrik/</t>
         </is>
       </c>
     </row>
@@ -6001,71 +6001,71 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Pyunik Yerevan</t>
+          <t>Alashkert</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Urartu</t>
+          <t>BKMA</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>1.66</v>
+        <v>1.33</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>24/10/2023 03:12</t>
+          <t>24/10/2023 00:12</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>1.61</v>
+        <v>1.36</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>25/10/2023 12:58</t>
+          <t>25/10/2023 12:51</t>
         </is>
       </c>
       <c r="N61" t="n">
-        <v>3.7</v>
+        <v>4.78</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>24/10/2023 03:12</t>
+          <t>24/10/2023 00:12</t>
         </is>
       </c>
       <c r="P61" t="n">
-        <v>3.92</v>
+        <v>4.99</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>25/10/2023 12:58</t>
+          <t>25/10/2023 12:51</t>
         </is>
       </c>
       <c r="R61" t="n">
-        <v>4.36</v>
+        <v>7.01</v>
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>24/10/2023 03:12</t>
+          <t>24/10/2023 00:12</t>
         </is>
       </c>
       <c r="T61" t="n">
-        <v>5.58</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>25/10/2023 12:58</t>
+          <t>25/10/2023 12:51</t>
         </is>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-urartu/tCTUlrik/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/alashkert-bkma/0Czsnty8/</t>
         </is>
       </c>
     </row>
@@ -7630,6 +7630,98 @@
       <c r="V78" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/armenia/premier-league/ararat-armenia-shirak-gyumri/YisIzklU/</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>45242.47916666666</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>2</v>
+      </c>
+      <c r="J79" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>10/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L79" t="n">
+        <v>8.449999999999999</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>12/11/2023 11:18</t>
+        </is>
+      </c>
+      <c r="N79" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>10/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P79" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>12/11/2023 11:18</t>
+        </is>
+      </c>
+      <c r="R79" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>10/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T79" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>12/11/2023 11:18</t>
+        </is>
+      </c>
+      <c r="V79" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/van-urartu/02k5wi4B/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 28-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V80"/>
+  <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5909,71 +5909,71 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Pyunik Yerevan</t>
+          <t>Alashkert</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Urartu</t>
+          <t>BKMA</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>1.66</v>
+        <v>1.33</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>24/10/2023 03:12</t>
+          <t>24/10/2023 00:12</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>1.61</v>
+        <v>1.36</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>25/10/2023 12:58</t>
+          <t>25/10/2023 12:51</t>
         </is>
       </c>
       <c r="N60" t="n">
-        <v>3.7</v>
+        <v>4.78</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>24/10/2023 03:12</t>
+          <t>24/10/2023 00:12</t>
         </is>
       </c>
       <c r="P60" t="n">
-        <v>3.92</v>
+        <v>4.99</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>25/10/2023 12:58</t>
+          <t>25/10/2023 12:51</t>
         </is>
       </c>
       <c r="R60" t="n">
-        <v>4.36</v>
+        <v>7.01</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>24/10/2023 03:12</t>
+          <t>24/10/2023 00:12</t>
         </is>
       </c>
       <c r="T60" t="n">
-        <v>5.58</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>25/10/2023 12:58</t>
+          <t>25/10/2023 12:51</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-urartu/tCTUlrik/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/alashkert-bkma/0Czsnty8/</t>
         </is>
       </c>
     </row>
@@ -6001,71 +6001,71 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Alashkert</t>
+          <t>Pyunik Yerevan</t>
         </is>
       </c>
       <c r="G61" t="n">
+        <v>3</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
         <v>1</v>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>BKMA</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>0</v>
-      </c>
       <c r="J61" t="n">
-        <v>1.33</v>
+        <v>1.66</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>24/10/2023 00:12</t>
+          <t>24/10/2023 03:12</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>1.36</v>
+        <v>1.61</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>25/10/2023 12:51</t>
+          <t>25/10/2023 12:58</t>
         </is>
       </c>
       <c r="N61" t="n">
-        <v>4.78</v>
+        <v>3.7</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>24/10/2023 00:12</t>
+          <t>24/10/2023 03:12</t>
         </is>
       </c>
       <c r="P61" t="n">
-        <v>4.99</v>
+        <v>3.92</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>25/10/2023 12:51</t>
+          <t>25/10/2023 12:58</t>
         </is>
       </c>
       <c r="R61" t="n">
-        <v>7.01</v>
+        <v>4.36</v>
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>24/10/2023 00:12</t>
+          <t>24/10/2023 03:12</t>
         </is>
       </c>
       <c r="T61" t="n">
-        <v>8.109999999999999</v>
+        <v>5.58</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>25/10/2023 12:51</t>
+          <t>25/10/2023 12:58</t>
         </is>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/alashkert-bkma/0Czsnty8/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-urartu/tCTUlrik/</t>
         </is>
       </c>
     </row>
@@ -7814,6 +7814,98 @@
       <c r="V80" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/armenia/premier-league/ararat-yerevan-alashkert/pQNNeYJu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>45258.625</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Shirak Gyumri</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Pyunik Yerevan</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="n">
+        <v>8.880000000000001</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>27/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L81" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>28/11/2023 13:46</t>
+        </is>
+      </c>
+      <c r="N81" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>27/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P81" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>28/11/2023 13:46</t>
+        </is>
+      </c>
+      <c r="R81" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>27/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T81" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>28/11/2023 13:26</t>
+        </is>
+      </c>
+      <c r="V81" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/shirak-gyumri-pyunik-yerevan/KrGzgW3b/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 29-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V81"/>
+  <dimension ref="A1:V82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7909,6 +7909,98 @@
         </is>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>45259.625</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Urartu</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>2</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Ararat Yerevan</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>28/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L82" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>29/11/2023 14:59</t>
+        </is>
+      </c>
+      <c r="N82" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>28/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P82" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>29/11/2023 14:59</t>
+        </is>
+      </c>
+      <c r="R82" t="n">
+        <v>6.04</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>28/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T82" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>29/11/2023 14:59</t>
+        </is>
+      </c>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/urartu-ararat-yerevan/OGMRfhZo/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 30-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/armenia_premier-league_2023-2024.xlsx
+++ b/2023/armenia_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V82"/>
+  <dimension ref="A1:V84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5449,22 +5449,22 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Pyunik Yerevan</t>
+          <t>Van</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Ararat-Armenia</t>
+          <t>Alashkert</t>
         </is>
       </c>
       <c r="I55" t="n">
         <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>1.85</v>
+        <v>6.34</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -5472,7 +5472,7 @@
         </is>
       </c>
       <c r="L55" t="n">
-        <v>1.99</v>
+        <v>7.32</v>
       </c>
       <c r="M55" t="inlineStr">
         <is>
@@ -5480,7 +5480,7 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>3.41</v>
+        <v>4.55</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -5488,7 +5488,7 @@
         </is>
       </c>
       <c r="P55" t="n">
-        <v>3.24</v>
+        <v>4.51</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -5496,7 +5496,7 @@
         </is>
       </c>
       <c r="R55" t="n">
-        <v>3.73</v>
+        <v>1.38</v>
       </c>
       <c r="S55" t="inlineStr">
         <is>
@@ -5504,7 +5504,7 @@
         </is>
       </c>
       <c r="T55" t="n">
-        <v>3.39</v>
+        <v>1.43</v>
       </c>
       <c r="U55" t="inlineStr">
         <is>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
         </is>
       </c>
     </row>
@@ -5541,22 +5541,22 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Van</t>
+          <t>Pyunik Yerevan</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Alashkert</t>
+          <t>Ararat-Armenia</t>
         </is>
       </c>
       <c r="I56" t="n">
         <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>6.34</v>
+        <v>1.85</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -5564,7 +5564,7 @@
         </is>
       </c>
       <c r="L56" t="n">
-        <v>7.32</v>
+        <v>1.99</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>4.55</v>
+        <v>3.41</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -5580,7 +5580,7 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>4.51</v>
+        <v>3.24</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -5588,7 +5588,7 @@
         </is>
       </c>
       <c r="R56" t="n">
-        <v>1.38</v>
+        <v>3.73</v>
       </c>
       <c r="S56" t="inlineStr">
         <is>
@@ -5596,7 +5596,7 @@
         </is>
       </c>
       <c r="T56" t="n">
-        <v>1.43</v>
+        <v>3.39</v>
       </c>
       <c r="U56" t="inlineStr">
         <is>
@@ -5605,7 +5605,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/armenia/premier-league/van-alashkert/S4mfepEL/</t>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/pyunik-yerevan-ararat-armenia/CxPQkOyq/</t>
         </is>
       </c>
     </row>
@@ -7998,6 +7998,190 @@
       <c r="V82" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/armenia/premier-league/urartu-ararat-yerevan/OGMRfhZo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>45260.47916666666</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Alashkert</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>1</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Ararat-Armenia</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>28/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L83" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>30/11/2023 11:21</t>
+        </is>
+      </c>
+      <c r="N83" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>28/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P83" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>30/11/2023 11:21</t>
+        </is>
+      </c>
+      <c r="R83" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>28/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T83" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>30/11/2023 11:21</t>
+        </is>
+      </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/alashkert-ararat-armenia/6uCWgClh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>45260.625</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>BKMA</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>7</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L84" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>30/11/2023 14:38</t>
+        </is>
+      </c>
+      <c r="N84" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P84" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>30/11/2023 14:38</t>
+        </is>
+      </c>
+      <c r="R84" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T84" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>30/11/2023 14:38</t>
+        </is>
+      </c>
+      <c r="V84" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/armenia/premier-league/bkma-van/hdEriAYA/</t>
         </is>
       </c>
     </row>

</xml_diff>